<commit_message>
Saved H1 Q1 Data
Saved the results of hypothesis 1 data with and without children into JSON format to prepare for the upcoming evaluation metrics.
</commit_message>
<xml_diff>
--- a/Excel-Files/Chi-Squared-Values/demo_question_chi_squared_values.xlsx
+++ b/Excel-Files/Chi-Squared-Values/demo_question_chi_squared_values.xlsx
@@ -458,7 +458,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -469,7 +469,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -480,7 +480,7 @@
         <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Produced Results DEMO H1
Hypothesis 1 demo results updated for people with and without children - 10 08 24. Further conditioning is required to improve the results.
</commit_message>
<xml_diff>
--- a/Excel-Files/Chi-Squared-Values/demo_question_chi_squared_values.xlsx
+++ b/Excel-Files/Chi-Squared-Values/demo_question_chi_squared_values.xlsx
@@ -491,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -502,7 +502,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
@@ -524,7 +524,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
@@ -535,7 +535,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
@@ -546,7 +546,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>